<commit_message>
Adding spreadsheet with performance data.
</commit_message>
<xml_diff>
--- a/PerformanceData.xlsx
+++ b/PerformanceData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="10">
   <si>
     <t>N points</t>
   </si>
@@ -218,10 +218,10 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>'20130410 - LineGraph'!$A$11:$A$18</c:f>
+              <c:f>'20130410 - LineGraph'!$A$11:$A$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
@@ -238,12 +238,15 @@
                   <c:v>100000</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>500000</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>1000000</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>10000000</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>50000000</c:v>
                 </c:pt>
               </c:numCache>
@@ -251,10 +254,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'20130410 - LineGraph'!$E$11:$E$18</c:f>
+              <c:f>'20130410 - LineGraph'!$E$11:$E$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>0.98078891934053503</c:v>
                 </c:pt>
@@ -271,12 +274,15 @@
                   <c:v>18.2812156718464</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>26.207897778505899</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>36.368197814545397</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>257.45137899999997</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>1178.12041129411</c:v>
                 </c:pt>
               </c:numCache>
@@ -292,11 +298,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="49702784"/>
-        <c:axId val="49701248"/>
+        <c:axId val="76518528"/>
+        <c:axId val="76520064"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="49702784"/>
+        <c:axId val="76518528"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -307,12 +313,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="49701248"/>
+        <c:crossAx val="76520064"/>
         <c:crossesAt val="0.1"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="49701248"/>
+        <c:axId val="76520064"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -324,7 +330,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="49702784"/>
+        <c:crossAx val="76518528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -668,10 +674,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -909,7 +915,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>1000000</v>
+        <v>500000</v>
       </c>
       <c r="B16" t="s">
         <v>5</v>
@@ -921,12 +927,12 @@
         <v>4</v>
       </c>
       <c r="E16">
-        <v>36.368197814545397</v>
+        <v>26.207897778505899</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>10000000</v>
+        <v>1000000</v>
       </c>
       <c r="B17" t="s">
         <v>5</v>
@@ -938,12 +944,12 @@
         <v>4</v>
       </c>
       <c r="E17">
-        <v>257.45137899999997</v>
+        <v>36.368197814545397</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18">
-        <v>50000000</v>
+        <v>10000000</v>
       </c>
       <c r="B18" t="s">
         <v>5</v>
@@ -955,6 +961,23 @@
         <v>4</v>
       </c>
       <c r="E18">
+        <v>257.45137899999997</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>50000000</v>
+      </c>
+      <c r="B19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E19">
         <v>1178.12041129411</v>
       </c>
     </row>

</xml_diff>